<commit_message>
BM25S Retriever Still WIP
</commit_message>
<xml_diff>
--- a/master_search_v0.xlsx
+++ b/master_search_v0.xlsx
@@ -1022,12 +1022,12 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
+          <t>Université de Lille [EPE]: Urbanisme et amenagement (inmp:1503363-19T)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
           <t>Université de La Réunion: Economie appliquée (inmp:1501143-05Y)</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Université Paris-X: Gestion de production, logistique, achats (inmp:1403146-04Z)</t>
         </is>
       </c>
       <c r="W6" t="inlineStr"/>
@@ -1292,30 +1292,34 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
+          <t>Université de Rennes: Microbiologie (inmp:1702406-03J)</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
           <t>Université de Caen Normandie: Mathématiques appliquées, statistique (inmp:1702210-01C)</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>Université Clermont Auvergne: Energie (inm:1702232C)</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>Université Grenoble Alpes: Génie civil (inmp:1603437-04K)</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Université de Pau: Géoénergies (inmp:1601699-06Z)</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>Ecole nationale supérieure de mécanique et d'aérotechnique de Poitiers: Aéronautique et espace (inmp:1801141-01X)</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
@@ -1452,7 +1456,11 @@
           <t>Université Paris-I: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), 2nd degré (inmp:1302615-27S)</t>
         </is>
       </c>
-      <c r="Y10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>Université de La Rochelle: Sciences et génie des matériaux (inmp:1502013-04M)</t>
+        </is>
+      </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
@@ -1644,7 +1652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -1683,6 +1691,14 @@
     <col width="100" customWidth="1" min="29" max="29"/>
     <col width="100" customWidth="1" min="30" max="30"/>
     <col width="100" customWidth="1" min="31" max="31"/>
+    <col width="100" customWidth="1" min="32" max="32"/>
+    <col width="100" customWidth="1" min="33" max="33"/>
+    <col width="100" customWidth="1" min="34" max="34"/>
+    <col width="100" customWidth="1" min="35" max="35"/>
+    <col width="100" customWidth="1" min="36" max="36"/>
+    <col width="100" customWidth="1" min="37" max="37"/>
+    <col width="100" customWidth="1" min="38" max="38"/>
+    <col width="100" customWidth="1" min="39" max="39"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1778,6 +1794,30 @@
       <c r="AE1" s="1" t="n">
         <v>29</v>
       </c>
+      <c r="AF1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1795,84 +1835,140 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Université Paris-XIII: Traitement automatique des langues (inmp:1405681-01P)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Université Paris Cité: Informatique fondamentale et appliquée (inmp:0901155-02H)</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Université de Bordeaux: Informatique (inmp:1603218-14S)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Université du Littoral: Langues, littératures et civilisations étrangères et régionales (inmp:1501948-01U)</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Université Aix-Marseille: Sciences cognitives (inmp:1800881-01L)</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Université de Toulon: Langues et sociétés (inmp:1800267-01X)</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Université de La Réunion: Français langue étrangère (inmp:1502960-01U)</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Histoire et philosophie des sciences (inmp:1405043-04V)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Université Paris Cité: Mathématiques et applications (inmp:1402116-20K)</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Université Grenoble Alpes: Mathématiques et informatique appliquées aux sciences humaines et sociales - MIASHS (inmp:1601750-10X)</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Université Toulouse-II: Lettres (inmp:1602412-01U)</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Université Paris Cité: Langues étrangères appliquées (inmp:0900894-03P)</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Université du Littoral: Ingénierie des systèmes complexes (inm:1501695C)</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Université Paris-XIII: Traitement automatique des langues (inmp:1405681-01P)</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Université Paris Cité: Histoire et philosophie des sciences (inmp:1405043-04V)</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1885,97 +1981,133 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Université de Montpellier: Physique fondamentale et applications (inmp:2200135-10V)</t>
+          <t>Nantes Université [EPE]: Physique fondamentale et applications (inmp:1702923-08K)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Ecole nationale supérieure d'ingénieurs de Caen: Ingénierie nucléaire (inm:2200151Q)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Université de Dijon: Physique (inmp:1701022-02Y)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>SORBONNE UNIVERSITE: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), 2nd degré (inmp:1302615-31W)</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Institut Polytechnique de Paris: Ingénierie nucléaire (inmp:1501525-11B)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>CY Cergy Paris Université: Physique (inmp:1503225-03A)</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Université de Poitiers: Sciences de la matière (inmp:1800795-05T)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Université de Montpellier: Sciences et numérique pour la santé (inmp:1501654-02N)</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Université Lyon-I: Génie des procédés et des bio-procédés (inmp:1601115-11B)</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Institut polytechnique de Grenoble: Sciences et génie des matériaux (inmp:1603028-15R)</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>SORBONNE UNIVERSITE: Mécanique (inmp:1900308-02V)</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Université de Poitiers: Sciences de la matière (inmp:1800795-05T)</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Université de Lorraine: Chimie (inm:1800173P)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Université de Poitiers: Energie (inmp:1800331-02E)</t>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Université de Rennes: Finance (inmp:1701983-12R)</t>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-16N)</t>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Ecole centrale de Lyon: Nanosciences et nanotechnologies (inmp:1601634-01D)</t>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Université de Nîmes: Risques et environnement (inmp:1502309-01H)</t>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Nantes Université [EPE]: Monnaie, banque, finance, assurance (inmp:1703248-03F)</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1988,22 +2120,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Université de La Réunion: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), 2nd degré (inmp:1501653-01D)</t>
+          <t>Institut Catholique de Toulouse: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), 2nd degré (inmp:2300050-01L)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>SORBONNE UNIVERSITE: Langues, littératures et civilisations étrangères et régionales (inmp:1900296-01P)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Université de Caen Normandie: Arts, lettres et civilisations (inmp:1702256-01C)</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Université du Littoral: Langues, littératures et civilisations étrangères et régionales (inmp:1501948-02V)</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Université Paris Est Créteil: Lettres (inmp:1502177-03M)</t>
+          <t>Université de Saint-Etienne: Lettres (inmp:1602346-11F)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -2011,20 +2143,76 @@
           <t>Université Paris Cité: Lettres et humanités (inmp:0900921-01X)</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -2035,6 +2223,14 @@
       <c r="AC4" t="inlineStr"/>
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2047,109 +2243,161 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Université de Bordeaux: Biologie-santé (inmp:1602061-02T)</t>
+          <t>SORBONNE UNIVERSITE: Biologie moléculaire et cellulaire (inmp:1900268-11G)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Université de Bordeaux: Biologie-santé (inmp:1602061-01S)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Université de Bordeaux: Chimie (inmp:1601500-03R)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Université de Poitiers: Ingénierie de la santé (inmp:1800779-02A)</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Ecole centrale de Nantes: Automatique, robotique (inmp:1702772-07W)</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Université Grenoble Alpes: Biologie (inmp:1602635-01H)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>Université de Lille [EPE]: Biotechnologies (inmp:1502725-03C)</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Université de Bordeaux: Biochimie, biologie moléculaire (inmp:1603091-01Y)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Ecole centrale de Nantes: Mécanique (inmp:1701739-10S)</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Université de Rennes: Biologie moléculaire et cellulaire (inmp:1702139-11W)</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Université de Caen Normandie: Sciences de la matière (inmp:1701899-05C)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Sciences du médicament et des produits de santé (inmp:1703372-18A)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>Université de Caen Normandie: Neurosciences (inmp:1703421-01H)</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Université de Rouen: Microbiologie (inmp:1701630-05N)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>Université de la Guyane: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), 2nd degré (inmp:1701784-05C)</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Université de Bordeaux: Archéologie, sciences pour l'archéologie (inmp:2200142-01W)</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Université de Rennes: Microbiologie (inmp:1702406-03J)</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Sciences du vivant (inmp:1800481-01H)</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>Université de Bordeaux: Biologie, agrosciences (inmp:1601934-11Y)</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Université de Bordeaux: Chimie (inmp:1601500-03R)</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Université Grenoble Alpes: Biologie (inmp:1602635-01H)</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Université de Caen Normandie: Sciences de la matière (inmp:1701899-05C)</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Nantes Université [EPE]: Sciences du médicament et des produits de santé (inmp:1703372-18A)</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>Université de Lorraine: Sciences du vivant (inm:1800178U)</t>
-        </is>
-      </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Université Grenoble Alpes: Biologie végétale (inmp:2100009-01Z)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Université Aix-Marseille: Biologie intégrative et physiologie (inmp:1800868-01Y)</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2162,149 +2410,169 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Université de Reims Champagne-Ardenne: Calcul haute performance, simulation (inmp:1800313-01X)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Université de Brest: Informatique (inmp:1702599-07S)</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Université Toulouse-III: Electronique, énergie électrique, automatique (inmp:1603154-07C)</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Université de Bordeaux: STAPS : entraînement et optimisation de la performance sportive (inmp:1602880-04S)</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Université de Besançon: Systèmes de calculs embarqués (inmp:1900374-02U)</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Avignon Université: Sciences et technologie de l'agriculture, de l'alimentation et de l'environnement (inmp:1801063-01U)</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Université Toulouse-III: Mathématiques et applications (inmp:1601717-10K)</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Université Clermont Auvergne: Automatique, robotique (inmp:1702216-01E)</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Université de Reims Champagne-Ardenne: STAPS : ingénierie et ergonomie de l'activité physique (inmp:1800323-01J)</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Université d'Angers: Marketing, vente (inmp:1701564-05P)</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>Université d'Amiens: Ingénierie de la santé (inmp:1801074-03S)</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>Institut national des sciences appliquées de Lyon: IA - Intelligence artificielle / AI - Artificial Intelligence (inm:2200132U)</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Université de technologie de Compiègne: Ingénierie des systèmes complexes (inmp:1201497-07H)</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>Université de Tours: Contrôle de gestion et audit organisationnel (inmp:1801083-01T)</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Université Paris-X: Sciences de l'éducation et de la formation (inmp:1402117-04B)</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>Ecole centrale de Nantes: Mécanique (inmp:1701739-10S)</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>Université de Chambéry: Management (inmp:1603064-26R)</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>Université Toulouse-III: Méthodes informatiques appliquées à la gestion des entreprises - MIAGE (inmp:1602749-17S)</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Urbanisme et amenagement (inmp:1503363-19T)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
         <is>
           <t>Université de La Réunion: Economie appliquée (inmp:1501143-05Y)</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>Université Paris-X: Gestion de production, logistique, achats (inmp:1403146-04Z)</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Université de Reims Champagne-Ardenne: Calcul haute performance, simulation (inmp:1800313-01X)</t>
-        </is>
-      </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>Université Bordeaux-III: Urbanisme et amenagement (inmp:1602941-01U)</t>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>Nantes Université [EPE]: Civilisations, cultures et sociétés (inmp:1703164-07E)</t>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>Ecole nationale supérieure d'architecture de Lyon: Ville et environnements urbains (inmp:1601862-19F)</t>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>Université Grenoble Alpes: Mathématiques et informatique appliquées aux sciences humaines et sociales - MIASHS (inmp:1601750-09W)</t>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>Université d'Angers: Direction de projets ou établissements culturels (inmp:1702530-05P)</t>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>Université d'Orléans: Mathématiques appliquées, statistique (inmp:1800490-01L)</t>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>Conservatoire national des arts et métiers: Gestion des ressources humaines (inmp:1604776-01A)</t>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>Nantes Université [EPE]: Droit de l'environnement et de l'urbanisme (inmp:1702654-02P)</t>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>Université Sorbonne Nouvelle - Paris 3: Traitement automatique des langues (inmp:1900179-04A)</t>
-        </is>
-      </c>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2382,44 +2650,84 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Université de Montpellier: Droit des affaires (inmp:2100077-02S)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Université de Montpellier: Droit de l'environnement (inmp:2100066-01V)</t>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Université de Lille [EPE]: Droit international et droit européen (inmp:2000209-01Y)</t>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Université de Rouen: Droit international (inmp:1703375-04L)</t>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>Institut catholique de Lyon: Droit des libertés (inmp:1602575-08U)</t>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>Université Clermont Auvergne: Droit notarial (inm:1701301R)</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2497,40 +2805,76 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Université Paris Cité: Sciences sociales (inmp:0900924-02Z)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Université de Dijon: Economie appliquée (inmp:1702433-04V)</t>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>Communauté d'universités et établissements Université Paris Lumières: Etudes politiques (inmp:1402045-02Y)</t>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Université de Besançon: Politiques publiques (inmp:2400096-01B)</t>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Université du Littoral: Didactique des langues (inmp:1502650-02Z)</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
       <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -2543,7 +2887,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Université Grenoble Alpes: Génie civil (inmp:1603437-04K)</t>
+          <t>Université Grenoble Alpes: Mécanique (inmp:1601777-02Y)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2553,95 +2897,147 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>SORBONNE UNIVERSITE: Physique fondamentale et applications (inmp:1900257-01A)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>Ecole nationale supérieure d'ingénieurs de Caen: Ingénierie nucléaire (inm:2200151Q)</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>SORBONNE UNIVERSITE: Mathématiques et applications (inmp:1900282-09B)</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>Université Paris Est Créteil: Chimie (inmp:1501718-05Y)</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Université de Lille [EPE]: Physique fondamentale et applications (inmp:2000176-02M)</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Université Paris-X: Génie industriel (inmp:1401838-02Y)</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>Université Grenoble Alpes: Physique (inmp:1602389-20P)</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Université de Poitiers: Mathématiques et applications (inmp:1800362-01Y)</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Université Grenoble Alpes: Génie des procédés et des bio-procédés (inmp:1602535-05T)</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>Université de Poitiers: Sciences de la matière (inmp:1800795-05T)</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Université Lyon-I: Génie des procédés et des bio-procédés (inmp:1601115-11B)</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>CY Cergy Paris Université: Sciences de la Terre et des planètes, environnement (inmp:1502274-06J)</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Université de Rennes: Microbiologie (inmp:1702406-03J)</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
         <is>
           <t>Université de Caen Normandie: Mathématiques appliquées, statistique (inmp:1702210-01C)</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>Université de Bordeaux: Mécanique (inmp:1602777-01T)</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Université de Pau: Géoénergies (inmp:1601699-06Z)</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Ecole nationale supérieure de mécanique et d'aérotechnique de Poitiers: Aéronautique et espace (inmp:1801141-01X)</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Université Paris-X: Génie industriel (inmp:1401838-02Y)</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Université de Pau: Géoénergies (inmp:1601699-06Z)</t>
-        </is>
-      </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>Université de Tours: Biologie-santé (inmp:1800443-01C)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Université de Tours: Informatique (inmp:1800406-03H)</t>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Université de Caen Normandie: Instrumentation, mesure, métrologie (inmp:2200099-01X)</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -2744,57 +3140,97 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
+          <t>Université de Montpellier: Energie (inmp:1501729-02R)</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
           <t>Université Paris Est Créteil: Administration et échanges internationaux (inmp:1503414-08Z)</t>
         </is>
       </c>
-      <c r="V10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>Université de Montpellier: Management (inmp:1502542-05N)</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="X10" t="inlineStr">
         <is>
           <t>Université Paris-I: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), 2nd degré (inmp:1302615-27S)</t>
         </is>
       </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>Université de la Guyane: Energie (inm:1501729P)</t>
-        </is>
-      </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>Ecole des hautes études en sciences sociales: Sociologie (inm:1900174Q)</t>
+          <t>Université de La Rochelle: Sciences et génie des matériaux (inmp:1502013-04M)</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Université Toulouse-III: Electronique, énergie électrique, automatique (inmp:1603154-03Y)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>Université de Corse: Risques et environnement (inmp:1801129-02U)</t>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>Université Grenoble Alpes: Ingénierie nucléaire (inmp:1603298-02Z)</t>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>Université Grenoble Alpes: Génie des procédés et des bio-procédés (inmp:1602535-05T)</t>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>Université Paris Cité: Histoire et philosophie des sciences (inmp:1405043-04V)</t>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>Université Paris Cité: Physique fondamentale et applications (inmp:0900816-11V)</t>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="AM10" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
         </is>
       </c>
     </row>
@@ -2814,50 +3250,74 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Université de Montpellier: Droit social (inmp:1503223-02G)</t>
+          <t>Université de Lille [EPE]: Marketing, vente (inmp:1501834-13R)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Université de Saint-Etienne: Droit des affaires (inmp:2200247-03L)</t>
+          <t>Université Paris Est Créteil: Science politique (inmp:1503073-08J)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Université de Rouen: Gestion des ressources humaines (inm:1701597M)</t>
+          <t>Université Paris 8: Humanités numériques (inmp:1502452-08J)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Université Paris-XIII: Communication des organisations (inmp:1505010-02W)</t>
+          <t>Institut catholique de Lille: Création numérique (inmp:2000066-08M)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Université de Corse: Management (inmp:1800401-01M)</t>
+          <t>Université de Lille [EPE]: Commerce et distribution (inmp:2000197-01U)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Conservatoire national des arts et métiers: Droit de l'entreprise (inm:1900196P)</t>
+          <t>Université de Montpellier: Management de l'innovation (inmp:1502491-02S)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Université de Rouen: Comptabilité - contrôle - audit (inm:1701896M)</t>
+          <t>Nantes Université [EPE]: Biologie-santé (inmp:1702149-15M)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Université de Lille [EPE]: Administration économique et sociale (inmp:1503383-02Y)</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+          <t>CY Cergy Paris Université: Métiers de l'enseignement, de l'éducation et de la formation (MEEF), pratiques et ingénierie de la formation (PIF) (inmp:1503069-43M)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Economie de l'entreprise et des marchés (inmp:2400101-01V)</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Université de Besançon: Langues étrangères appliquées (inmp:1702067-02K)</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Université Paris Est Créteil: Entrepreneuriat et management de projets (inmp:1501795-01N)</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Université d'Orléans: Econométrie, statistiques (inmp:1800493-01M)</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Université Paris Cité: Informatique (inmp:1004670-08V)</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Conservatoire national des arts et métiers: Audiovisuel, médias interactifs numériques, jeux (inmp:1604791-06L)</t>
+        </is>
+      </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -2872,6 +3332,14 @@
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>